<commit_message>
updated manage/add categories layout
</commit_message>
<xml_diff>
--- a/docs/Work_log.xlsx
+++ b/docs/Work_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\upwork\FED\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1A0E3F-7D77-4847-A52A-A2A969C9C03D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794D3E33-35D1-4278-B9FE-F6D1D960787D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{9644458F-0DAE-45AA-9529-3FF0F1BC5289}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{9644458F-0DAE-45AA-9529-3FF0F1BC5289}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>Login</t>
   </si>
@@ -458,23 +458,23 @@
   <dimension ref="B7:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D13" sqref="D13:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="9.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="1"/>
     <col min="4" max="4" width="32" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.88671875" style="1"/>
-    <col min="8" max="8" width="21.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
@@ -500,7 +500,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>1</v>
       </c>
@@ -520,7 +520,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="1">
         <v>2</v>
@@ -531,8 +531,11 @@
       <c r="F9" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="G9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="1">
         <v>3</v>
@@ -543,8 +546,11 @@
       <c r="F10" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="G10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="1">
         <v>4</v>
@@ -555,8 +561,11 @@
       <c r="F11" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="G11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="1">
         <v>5</v>
@@ -571,7 +580,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="1">
         <v>6</v>
@@ -583,7 +592,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="1">
         <v>7</v>
@@ -595,7 +604,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="1">
         <v>8</v>
@@ -607,7 +616,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="1">
         <v>9</v>
@@ -619,7 +628,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="1">
         <v>10</v>

</xml_diff>